<commit_message>
Updated USM to only have essential items in the first release
</commit_message>
<xml_diff>
--- a/Deliverable 3/USM Map.xlsx
+++ b/Deliverable 3/USM Map.xlsx
@@ -65,6 +65,15 @@
     <t>Give prompts in app for kids to answer</t>
   </si>
   <si>
+    <t>Develop prompt interface that guides parents through questions</t>
+  </si>
+  <si>
+    <t>Release 2</t>
+  </si>
+  <si>
+    <t>Point system is added to app to gamify it.</t>
+  </si>
+  <si>
     <t>Make 911 simulation app downloadable</t>
   </si>
   <si>
@@ -74,25 +83,16 @@
     <t>Create list interface to show questions and appropriate responses.</t>
   </si>
   <si>
+    <t>Display additional fire safety info in app</t>
+  </si>
+  <si>
+    <t>Link to app is accessible and app is downloadable through email</t>
+  </si>
+  <si>
+    <t>Display the list of questions that 911 operators will ask</t>
+  </si>
+  <si>
     <t>Create readable structure for additional information</t>
-  </si>
-  <si>
-    <t>Develop prompt interface that guides parents through questions</t>
-  </si>
-  <si>
-    <t>Point system is added to app to gamify it.</t>
-  </si>
-  <si>
-    <t>Display the list of questions that 911 operators will ask</t>
-  </si>
-  <si>
-    <t>Display additional fire safety info in app</t>
-  </si>
-  <si>
-    <t>Release 2</t>
-  </si>
-  <si>
-    <t>Link to app is accessible and app is downloadable through email</t>
   </si>
   <si>
     <t>Release 3 (Down the line)</t>
@@ -337,61 +337,61 @@
       <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="T7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="5" t="s">
+    </row>
+    <row r="8" ht="10" customHeight="1"/>
+    <row r="9">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" ht="10" customHeight="1"/>
+    <row r="11" ht="72" customHeight="1">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" ht="10" customHeight="1"/>
-    <row r="9" ht="72" customHeight="1">
-      <c r="D9" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="R11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" ht="10" customHeight="1"/>
-    <row r="11">
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
     </row>
     <row r="12" ht="10" customHeight="1"/>
     <row r="13" ht="72" customHeight="1">
       <c r="N13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>